<commit_message>
Fix AuthContext setInitialLoadComplete error and implement spreadsheet import functionality
</commit_message>
<xml_diff>
--- a/backend/estudantes_ficticios_corrigido (1).xlsx
+++ b/backend/estudantes_ficticios_corrigido (1).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/696b7a661993207c/Documents/GitHub/ministry-hub-sync/backend/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\webbe\Documents\GitHub\ministry-hub-sync\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A116038-1027-426B-B1F1-CF6B6E9B0273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E24B4D5-4F6A-4993-928E-AC34DFAE6A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2328,11 +2328,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection sqref="A1:AI101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="34" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>